<commit_message>
importation réussie de 73 sites et 511 tâches
</commit_message>
<xml_diff>
--- a/fichier_sites.xlsx
+++ b/fichier_sites.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -79,7 +79,7 @@
     <t xml:space="preserve">EXT L800</t>
   </si>
   <si>
-    <t xml:space="preserve">2279  + 4415</t>
+    <t xml:space="preserve">2279 + 4415</t>
   </si>
   <si>
     <t xml:space="preserve">GLODJIGBE_2</t>
@@ -326,6 +326,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -347,6 +348,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -360,13 +362,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -449,56 +451,64 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -687,8 +697,8 @@
   </sheetPr>
   <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G46" activeCellId="0" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -747,13 +757,13 @@
       <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -776,13 +786,13 @@
       <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -802,16 +812,16 @@
       <c r="F4" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -831,16 +841,16 @@
       <c r="F5" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="0" t="n">
+      <c r="H5" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="0" t="n">
+      <c r="J5" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -860,16 +870,16 @@
       <c r="F6" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="0" t="n">
+      <c r="H6" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -889,16 +899,16 @@
       <c r="F7" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H7" s="0" t="n">
+      <c r="H7" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="0" t="n">
+      <c r="J7" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -921,16 +931,16 @@
       <c r="G8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="0" t="n">
+      <c r="H8" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J8" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K8" s="0" t="n">
+      <c r="J8" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K8" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -953,16 +963,16 @@
       <c r="G9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H9" s="0" t="n">
+      <c r="H9" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K9" s="0" t="n">
+      <c r="J9" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K9" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -985,16 +995,16 @@
       <c r="G10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="0" t="n">
+      <c r="H10" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J10" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K10" s="0" t="n">
+      <c r="J10" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K10" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -1014,16 +1024,16 @@
       <c r="F11" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="0" t="n">
+      <c r="H11" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J11" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1043,16 +1053,16 @@
       <c r="F12" s="6" t="n">
         <v>44621</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H12" s="0" t="n">
+      <c r="H12" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="0" t="n">
+      <c r="J12" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1075,13 +1085,13 @@
       <c r="G13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H13" s="0" t="n">
+      <c r="H13" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J13" s="0" t="n">
+      <c r="J13" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1104,13 +1114,13 @@
       <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="0" t="n">
+      <c r="H14" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="0" t="n">
+      <c r="J14" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1133,13 +1143,13 @@
       <c r="G15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="0" t="n">
+      <c r="H15" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J15" s="0" t="n">
+      <c r="J15" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1162,13 +1172,13 @@
       <c r="G16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H16" s="0" t="n">
+      <c r="H16" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J16" s="0" t="n">
+      <c r="J16" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1191,13 +1201,13 @@
       <c r="G17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H17" s="0" t="n">
+      <c r="H17" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J17" s="0" t="n">
+      <c r="J17" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1220,13 +1230,13 @@
       <c r="G18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H18" s="0" t="n">
+      <c r="H18" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="0" t="n">
+      <c r="J18" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1249,13 +1259,13 @@
       <c r="G19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="0" t="n">
+      <c r="H19" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="0" t="n">
+      <c r="J19" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1278,13 +1288,13 @@
       <c r="G20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H20" s="0" t="n">
+      <c r="H20" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J20" s="0" t="n">
+      <c r="J20" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1307,13 +1317,13 @@
       <c r="G21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H21" s="0" t="n">
+      <c r="H21" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J21" s="0" t="n">
+      <c r="J21" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1336,13 +1346,13 @@
       <c r="G22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="0" t="n">
+      <c r="H22" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J22" s="0" t="n">
+      <c r="J22" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1365,13 +1375,13 @@
       <c r="G23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="0" t="n">
+      <c r="H23" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J23" s="0" t="n">
+      <c r="J23" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1394,13 +1404,13 @@
       <c r="G24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H24" s="0" t="n">
+      <c r="H24" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="0" t="n">
+      <c r="J24" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1423,16 +1433,16 @@
       <c r="G25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="0" t="n">
+      <c r="H25" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J25" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K25" s="0" t="n">
+      <c r="J25" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K25" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -1455,16 +1465,16 @@
       <c r="G26" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="0" t="n">
+      <c r="H26" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K26" s="0" t="n">
+      <c r="J26" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K26" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -1487,24 +1497,24 @@
       <c r="G27" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="H27" s="0" t="n">
+      <c r="H27" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K27" s="0" t="n">
+      <c r="J27" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K27" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="9" t="s">
         <v>49</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -1519,21 +1529,21 @@
       <c r="G28" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H28" s="0" t="n">
+      <c r="H28" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J28" s="0" t="n">
+      <c r="J28" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="9" t="s">
         <v>50</v>
       </c>
       <c r="C29" s="4" t="s">
@@ -1548,21 +1558,21 @@
       <c r="G29" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H29" s="0" t="n">
+      <c r="H29" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J29" s="0" t="n">
+      <c r="J29" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="9" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -1577,21 +1587,21 @@
       <c r="G30" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H30" s="0" t="n">
+      <c r="H30" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J30" s="0" t="n">
+      <c r="J30" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="9" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1606,21 +1616,21 @@
       <c r="G31" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H31" s="0" t="n">
+      <c r="H31" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J31" s="0" t="n">
+      <c r="J31" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -1635,21 +1645,21 @@
       <c r="G32" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="0" t="n">
+      <c r="H32" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I32" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J32" s="0" t="n">
+      <c r="J32" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -1664,13 +1674,13 @@
       <c r="G33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H33" s="0" t="n">
+      <c r="H33" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J33" s="0" t="n">
+      <c r="J33" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1693,13 +1703,13 @@
       <c r="G34" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="0" t="n">
+      <c r="H34" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I34" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J34" s="0" t="n">
+      <c r="J34" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1722,13 +1732,13 @@
       <c r="G35" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="0" t="n">
+      <c r="H35" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J35" s="0" t="n">
+      <c r="J35" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1751,27 +1761,27 @@
       <c r="G36" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H36" s="0" t="n">
+      <c r="H36" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J36" s="0" t="n">
+      <c r="J36" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="6" t="n">
@@ -1780,13 +1790,13 @@
       <c r="G37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H37" s="0" t="n">
+      <c r="H37" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J37" s="0" t="n">
+      <c r="J37" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1809,13 +1819,13 @@
       <c r="G38" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H38" s="0" t="n">
+      <c r="H38" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J38" s="0" t="n">
+      <c r="J38" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1838,13 +1848,13 @@
       <c r="G39" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H39" s="0" t="n">
+      <c r="H39" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J39" s="0" t="n">
+      <c r="J39" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1867,13 +1877,13 @@
       <c r="G40" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="0" t="n">
+      <c r="H40" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J40" s="0" t="n">
+      <c r="J40" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1896,13 +1906,13 @@
       <c r="G41" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="0" t="n">
+      <c r="H41" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J41" s="0" t="n">
+      <c r="J41" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1925,13 +1935,13 @@
       <c r="G42" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H42" s="0" t="n">
+      <c r="H42" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J42" s="0" t="n">
+      <c r="J42" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1954,13 +1964,13 @@
       <c r="G43" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H43" s="0" t="n">
+      <c r="H43" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I43" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J43" s="0" t="n">
+      <c r="J43" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -1984,13 +1994,13 @@
       <c r="G44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H44" s="0" t="n">
+      <c r="H44" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J44" s="0" t="n">
+      <c r="J44" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2010,19 +2020,19 @@
       <c r="F45" s="6" t="n">
         <v>44713</v>
       </c>
-      <c r="G45" s="5" t="s">
+      <c r="G45" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H45" s="0" t="n">
+      <c r="H45" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J45" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K45" s="0" t="n">
+      <c r="J45" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K45" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -2042,46 +2052,46 @@
       <c r="F46" s="6" t="n">
         <v>44713</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="G46" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H46" s="0" t="n">
+      <c r="H46" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J46" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K46" s="0" t="n">
+      <c r="J46" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K46" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="11" t="s">
         <v>69</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="9"/>
+      <c r="D47" s="11"/>
       <c r="F47" s="6" t="n">
         <v>44713</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H47" s="0" t="n">
+      <c r="H47" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I47" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J47" s="0" t="n">
+      <c r="J47" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2102,13 +2112,13 @@
       <c r="G48" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H48" s="0" t="n">
+      <c r="H48" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I48" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J48" s="0" t="n">
+      <c r="J48" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2129,13 +2139,13 @@
       <c r="G49" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H49" s="0" t="n">
+      <c r="H49" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J49" s="0" t="n">
+      <c r="J49" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2156,13 +2166,13 @@
       <c r="G50" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H50" s="0" t="n">
+      <c r="H50" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J50" s="0" t="n">
+      <c r="J50" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2183,13 +2193,13 @@
       <c r="G51" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H51" s="0" t="n">
+      <c r="H51" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I51" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J51" s="0" t="n">
+      <c r="J51" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2210,13 +2220,13 @@
       <c r="G52" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H52" s="0" t="n">
+      <c r="H52" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I52" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J52" s="0" t="n">
+      <c r="J52" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2237,13 +2247,13 @@
       <c r="G53" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H53" s="0" t="n">
+      <c r="H53" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I53" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J53" s="0" t="n">
+      <c r="J53" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2264,13 +2274,13 @@
       <c r="G54" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H54" s="0" t="n">
+      <c r="H54" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I54" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J54" s="0" t="n">
+      <c r="J54" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2291,13 +2301,13 @@
       <c r="G55" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H55" s="0" t="n">
+      <c r="H55" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I55" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J55" s="0" t="n">
+      <c r="J55" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2318,13 +2328,13 @@
       <c r="G56" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H56" s="0" t="n">
+      <c r="H56" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I56" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J56" s="0" t="n">
+      <c r="J56" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2347,13 +2357,13 @@
       <c r="G57" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H57" s="0" t="n">
+      <c r="H57" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J57" s="0" t="n">
+      <c r="J57" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2376,13 +2386,13 @@
       <c r="G58" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H58" s="0" t="n">
+      <c r="H58" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I58" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J58" s="0" t="n">
+      <c r="J58" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2405,13 +2415,13 @@
       <c r="G59" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H59" s="0" t="n">
+      <c r="H59" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J59" s="0" t="n">
+      <c r="J59" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2434,13 +2444,13 @@
       <c r="G60" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H60" s="0" t="n">
+      <c r="H60" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I60" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J60" s="0" t="n">
+      <c r="J60" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2463,13 +2473,13 @@
       <c r="G61" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H61" s="0" t="n">
+      <c r="H61" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I61" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J61" s="0" t="n">
+      <c r="J61" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2492,21 +2502,21 @@
       <c r="G62" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H62" s="0" t="n">
+      <c r="H62" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I62" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J62" s="0" t="n">
+      <c r="J62" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+      <c r="A63" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B63" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C63" s="4" t="s">
@@ -2521,13 +2531,13 @@
       <c r="G63" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H63" s="0" t="n">
+      <c r="H63" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I63" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J63" s="0" t="n">
+      <c r="J63" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2550,13 +2560,13 @@
       <c r="G64" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H64" s="0" t="n">
+      <c r="H64" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J64" s="0" t="n">
+      <c r="J64" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2579,21 +2589,21 @@
       <c r="G65" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H65" s="0" t="n">
+      <c r="H65" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J65" s="0" t="n">
+      <c r="J65" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+      <c r="A66" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B66" s="12" t="s">
         <v>88</v>
       </c>
       <c r="C66" s="4" t="s">
@@ -2608,13 +2618,13 @@
       <c r="G66" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H66" s="0" t="n">
+      <c r="H66" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I66" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J66" s="0" t="n">
+      <c r="J66" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2637,13 +2647,13 @@
       <c r="G67" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H67" s="0" t="n">
+      <c r="H67" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J67" s="0" t="n">
+      <c r="J67" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2666,13 +2676,13 @@
       <c r="G68" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H68" s="0" t="n">
+      <c r="H68" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I68" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J68" s="0" t="n">
+      <c r="J68" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2695,13 +2705,13 @@
       <c r="G69" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H69" s="0" t="n">
+      <c r="H69" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I69" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J69" s="0" t="n">
+      <c r="J69" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2724,13 +2734,13 @@
       <c r="G70" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H70" s="0" t="n">
+      <c r="H70" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I70" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J70" s="0" t="n">
+      <c r="J70" s="7" t="n">
         <v>6630</v>
       </c>
     </row>
@@ -2750,19 +2760,19 @@
       <c r="F71" s="6" t="n">
         <v>44743</v>
       </c>
-      <c r="G71" s="5" t="s">
+      <c r="G71" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H71" s="0" t="n">
+      <c r="H71" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I71" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J71" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K71" s="0" t="n">
+      <c r="J71" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K71" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -2782,27 +2792,27 @@
       <c r="F72" s="6" t="n">
         <v>44743</v>
       </c>
-      <c r="G72" s="5" t="s">
+      <c r="G72" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H72" s="0" t="n">
+      <c r="H72" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I72" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J72" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K72" s="0" t="n">
+      <c r="J72" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K72" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C73" s="4" t="s">
@@ -2814,19 +2824,19 @@
       <c r="F73" s="6" t="n">
         <v>44743</v>
       </c>
-      <c r="G73" s="5" t="s">
+      <c r="G73" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H73" s="0" t="n">
+      <c r="H73" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I73" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J73" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K73" s="0" t="n">
+      <c r="J73" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K73" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
@@ -2846,24 +2856,24 @@
       <c r="F74" s="6" t="n">
         <v>44743</v>
       </c>
-      <c r="G74" s="5" t="s">
+      <c r="G74" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H74" s="0" t="n">
+      <c r="H74" s="7" t="n">
         <v>3</v>
       </c>
       <c r="I74" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J74" s="0" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K74" s="0" t="n">
+      <c r="J74" s="7" t="n">
+        <v>6630</v>
+      </c>
+      <c r="K74" s="7" t="n">
         <v>6150</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G75" s="12"/>
+      <c r="G75" s="14"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>